<commit_message>
update on 20210731 画中人
</commit_message>
<xml_diff>
--- a/story/Activity Story 活动剧情/a001 Grani and the Knights' Treasure 骑兵与猎人 騎兵と狩人/level_a001_01_beg.xlsx
+++ b/story/Activity Story 活动剧情/a001 Grani and the Knights' Treasure 骑兵与猎人 騎兵と狩人/level_a001_01_beg.xlsx
@@ -848,7 +848,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[name=""]   Clear \ Visibility: 14 km 
+    <t xml:space="preserve">[name=""]   Clear \ Visibility: 14 km 
 </t>
   </si>
   <si>
@@ -1000,7 +1000,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[name="Carol"]   ...All because of those "Knights' Treasures."
+    <t xml:space="preserve">[name="Carol"]   ...All because of those 'Knights' Treasures.'
 </t>
   </si>
   <si>
@@ -1032,11 +1032,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[name="Carol"]   "The ancient Knights of Kazimierz were all buried with their riches near the lands they once called home. Their souls protect these unmarked graves for all of eternity."
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[name="Carol"]   "Only those who fear not sacrifice and possess the true, dauntless bloodline of Kazimierz may open the path."
+    <t xml:space="preserve">[name="Carol"]   'The ancient Knights of Kazimierz were all buried with their riches near the lands they once called home. Their souls protect these unmarked graves for all of eternity.'
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Carol"]   'Only those who fear not sacrifice and possess the true, dauntless bloodline of Kazimierz may open the path.'
 </t>
   </si>
   <si>

</xml_diff>